<commit_message>
correctionregex et ajout fichier test
</commit_message>
<xml_diff>
--- a/Plan test.xlsx
+++ b/Plan test.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="76">
   <si>
     <t>Fichier JS</t>
   </si>
@@ -37,19 +37,34 @@
     <t>index.js</t>
   </si>
   <si>
-    <t>1-29</t>
-  </si>
-  <si>
-    <t>fetch</t>
-  </si>
-  <si>
-    <t>La requête doit retourner tous les articles disponibles à la vente présent sur l'API</t>
-  </si>
-  <si>
-    <t>ouvrir la page index.html et comparer les informations contenues sur cette page avec les informations contenues sur l'API</t>
-  </si>
-  <si>
-    <t xml:space="preserve">La valeur retournée pourrait être érronée </t>
+    <t>4-8</t>
+  </si>
+  <si>
+    <t>function(response)</t>
+  </si>
+  <si>
+    <t>récupère la réponse du serveur sous format JSON</t>
+  </si>
+  <si>
+    <t xml:space="preserve">faire un console.log(response.json) </t>
+  </si>
+  <si>
+    <t>La requête pourrait contenir un chemin erroné ou le serveur pourrait ne pas avoir été lancé</t>
+  </si>
+  <si>
+    <t>10-27</t>
+  </si>
+  <si>
+    <t>function (listOfProducts)</t>
+  </si>
+  <si>
+    <t>Récupère tous les articles disponibles sur l'API et les affiche dynamiquement sous forme de liste sur le DOM</t>
+  </si>
+  <si>
+    <t>faire un console.log (listOfProducts) et comparer les informations contenues sur la page index.html avec les informations contenues sur l'API</t>
+  </si>
+  <si>
+    <t>un des identifiants</t>
   </si>
   <si>
     <t>16</t>
@@ -64,79 +79,78 @@
     <t>Le paramètre de l'URL de la page de l'article doit correspondre à L'id de l'article cliqué</t>
   </si>
   <si>
-    <t>La page ouverte pourrai tne pas correspondre à l'article cliqué</t>
+    <t>Le chemin de l'url pourrait être erronné, la page ouverte pourrait ne pas correspondre à l'article selectionner</t>
   </si>
   <si>
     <t>article.js</t>
   </si>
   <si>
-    <t>2</t>
-  </si>
-  <si>
-    <t>getParameters</t>
-  </si>
-  <si>
-    <t>récupère l'id de article contenu dans l'URL</t>
-  </si>
-  <si>
-    <t>Faire un console.log(getParameters) et vérifier que le réusltat correspond bien à l'identifiant de l'article concerné</t>
-  </si>
-  <si>
-    <t>oublie de caractère à remplacer pour faire fonctionner obter l'id de l'article</t>
-  </si>
-  <si>
-    <t>6</t>
-  </si>
-  <si>
-    <t>fetch(`http://localhost:3000/api/teddies/${getParameters}`)</t>
-  </si>
-  <si>
-    <t>recupération des informations de l'article concerné en fonction de son id</t>
-  </si>
-  <si>
-    <t>      Faire un  console.log (article) et vérifier que les informations de l'article correspondent bien aux information de l'article cliqué</t>
+    <t>8-12</t>
+  </si>
+  <si>
+    <t>  function(response)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">récupère la réponse du serveur avec l'id en paramètre sous format JSON </t>
+  </si>
+  <si>
+    <t>14-104</t>
+  </si>
+  <si>
+    <t>function (article)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Récupère et utilise les informations de l'article concerné en fonction de son id et l'afiche dynamiquement sur le DOM </t>
+  </si>
+  <si>
+    <t>Faire un  console.log (article) et vérifier que les informations de l'article correspondent bien aux informations de l'article cliqué</t>
   </si>
   <si>
     <t>La requète pourrait ne pas avoir le bon format, ne pas fonctionner ou pourrait retourner des informations erronées</t>
   </si>
   <si>
-    <t>29</t>
-  </si>
-  <si>
-    <t>for (let color of article.colors){</t>
-  </si>
-  <si>
-    <t>boucle permetant d'afficher toutes les couleurs disponibles pour chaque article</t>
-  </si>
-  <si>
     <t>61</t>
   </si>
   <si>
     <t>function showcolor()</t>
   </si>
   <si>
-    <t xml:space="preserve">permet de récupérer la couleur selectionnée </t>
+    <t>permet de récupérer la couleur selectionnée par l'utilisateur</t>
+  </si>
+  <si>
+    <t>Appeller la fonction avec différentes valeurs de tests, et on observe la valeur retournée, avec un console.log(getcolorSelected)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">La valeur retournée pourrait être érronée
+</t>
   </si>
   <si>
     <t>71</t>
   </si>
   <si>
-    <t> function showquantity(){</t>
-  </si>
-  <si>
-    <t>83-99</t>
-  </si>
-  <si>
-    <t>btnAddCart.addEventListener("cliquek",function()</t>
-  </si>
-  <si>
-    <t>au clique sur le bouton "ajouter au panier":
-1-récupérer les informations liées à l'article et les stocker dans le local storage
-2- réupérer la quantité et la couleur selectionnées
-3-si le locale storage n'est pas vide, ajout de l'article selectionné dans dans le locale storage, si le locale storage est vide, creer un array panier dans lequel on ajoute l'article selectionné</t>
-  </si>
-  <si>
-    <t>console.log(selectedArticle);</t>
+    <t> function showquantity()</t>
+  </si>
+  <si>
+    <t>permet de récupérer la quantité selectionnée par l'utilisateur</t>
+  </si>
+  <si>
+    <t>Appeller la fonction avec différentes valeurs de tests, et on observe la valeur retournée, avec un console.log(getQuantitySelected)</t>
+  </si>
+  <si>
+    <t>83-100</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    btnAddCart.addEventListener("click",function()
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">au clic sur le bouton "ajouter au panier", récupérer les informations lié à l'article et à sa personnalisation pour les stocker dans le locale storage et afficher une pop up confirmant l'ajout de l'article au panier </t>
+  </si>
+  <si>
+    <t>Appeller la fonction avec différentes valeurs de tests (ex: ajouter différent articles ou ajouter différentes couleurs et quantités au même arrticle), et on observe la valeur retournée, avec un console.log(      console.log(selectedArticle), puis vérifier que ces éléments sont bien stockés dans le locale storage via l'onglet Application du devtool</t>
+  </si>
+  <si>
+    <t xml:space="preserve">les articles ne sont pas stockés au locale storage ou les élements de personnalisation ne sont pas pris en compte </t>
   </si>
   <si>
     <t>97-104</t>
@@ -145,7 +159,13 @@
     <t>close popup</t>
   </si>
   <si>
-    <t>afficher la popup lorsque l'utilisateur clique sur "ajouter au panier" puis fermer la pop up lorsque qu'il clique sur le bouton X</t>
+    <t>ferme la pop up lorsque l'utilisateur clique sur le bouton X</t>
+  </si>
+  <si>
+    <t>appuyer sur la croix de la pop up et vérifier qu'elle se ferme bien</t>
+  </si>
+  <si>
+    <t>la fenêtre pourrait ne pas se fermer dans la cas d'une erreur de code</t>
   </si>
   <si>
     <t>shoppingcart.js</t>
@@ -169,7 +189,7 @@
     <t>transforme les données json en javascript</t>
   </si>
   <si>
-    <t>7-41</t>
+    <t>11-45</t>
   </si>
   <si>
     <t>document.addEventListener("DOMContentLoaded", function(event)</t>
@@ -177,10 +197,55 @@
   <si>
     <t>une fois la page chargé, afficher la liste des articles contenus dans le locale storage (bloucle for ...of)
 2-calculer le prix total du panier 
-3-</t>
+3-afficher dynamiquement les informations liés aux articles ajoutés au panier</t>
+  </si>
+  <si>
+    <t>ajouter plusieurs articles différents au panier et vérifier qu'ils s'affichent bien et que les monant s'actualisent bien</t>
+  </si>
+  <si>
+    <t>tous les articles ajoutés au panier ne s'affichent pas, le prix total du panier ne s'affiche pas (si par exemple les données sont de type string et pas number) ou ne s'actualise pas (s'il n'y a pas de boucle êrmettant d'additionner le prx de chaque article du panier par exemple)</t>
+  </si>
+  <si>
+    <t>47-57</t>
+  </si>
+  <si>
+    <t>function deleteArticle(i)</t>
+  </si>
+  <si>
+    <t>85-155</t>
+  </si>
+  <si>
+    <t>myForm.addEventListener('submit',function(e)</t>
+  </si>
+  <si>
+    <t>123-155</t>
+  </si>
+  <si>
+    <t>function send(e)</t>
+  </si>
+  <si>
+    <t>144-148</t>
+  </si>
+  <si>
+    <t>149-152</t>
+  </si>
+  <si>
+    <t>function (orderid)</t>
   </si>
   <si>
     <t>orderconfirmation.js</t>
+  </si>
+  <si>
+    <t>1-12</t>
+  </si>
+  <si>
+    <t>document.addEventListener("DOMContentLoaded", function(event) </t>
+  </si>
+  <si>
+    <t>15-17</t>
+  </si>
+  <si>
+    <t>window.addEventListener("beforeunload", function (e) </t>
   </si>
 </sst>
 </file>
@@ -188,10 +253,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="176" formatCode="_-&quot;€&quot;* #,##0_-;\-&quot;€&quot;* #,##0_-;_-&quot;€&quot;* \-_-;_-@_-"/>
+    <numFmt numFmtId="177" formatCode="_-&quot;€&quot;* #,##0.00_-;\-&quot;€&quot;* #,##0.00_-;_-&quot;€&quot;* \-??_-;_-@_-"/>
     <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="176" formatCode="_-&quot;€&quot;* #,##0_-;\-&quot;€&quot;* #,##0_-;_-&quot;€&quot;* \-_-;_-@_-"/>
-    <numFmt numFmtId="177" formatCode="_-&quot;€&quot;* #,##0.00_-;\-&quot;€&quot;* #,##0.00_-;_-&quot;€&quot;* \-??_-;_-@_-"/>
   </numFmts>
   <fonts count="21">
     <font>
@@ -210,14 +275,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -225,16 +283,9 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -246,6 +297,21 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="13"/>
       <color theme="3"/>
@@ -254,6 +320,43 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
@@ -262,11 +365,10 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -286,50 +388,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF0000FF"/>
@@ -339,7 +397,14 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -397,25 +462,103 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFCC99"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
+        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -427,6 +570,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -439,13 +588,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -469,90 +624,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFC6EFCE"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -566,12 +637,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -600,6 +665,69 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
       <top style="thin">
@@ -621,21 +749,6 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
         <color rgb="FF7F7F7F"/>
       </left>
       <right style="thin">
@@ -649,60 +762,12 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -720,130 +785,130 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="9" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="22" borderId="9" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="23" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1045,8 +1110,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:F27" totalsRowShown="0">
-  <autoFilter ref="A1:F27"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:F20" totalsRowShown="0">
+  <autoFilter ref="A1:F20"/>
   <tableColumns count="6">
     <tableColumn id="1" name="Fichier JS" dataDxfId="0"/>
     <tableColumn id="2" name="Lignes de code testées" dataDxfId="1"/>
@@ -1317,20 +1382,21 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:F27"/>
+  <dimension ref="A1:F20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="D18" sqref="D18"/>
+      <selection pane="bottomLeft" activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelCol="5"/>
   <cols>
     <col min="1" max="1" width="20" customWidth="1"/>
     <col min="2" max="2" width="22.1428571428571" customWidth="1"/>
-    <col min="3" max="3" width="25.8571428571429" customWidth="1"/>
-    <col min="4" max="5" width="31.8571428571429" customWidth="1"/>
+    <col min="3" max="3" width="34" customWidth="1"/>
+    <col min="4" max="4" width="31.8571428571429" customWidth="1"/>
+    <col min="5" max="5" width="39.1428571428571" customWidth="1"/>
     <col min="6" max="6" width="43.1428571428571" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1354,7 +1420,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" ht="60" spans="1:6">
+    <row r="2" ht="30" spans="1:6">
       <c r="A2" s="3" t="s">
         <v>6</v>
       </c>
@@ -1374,7 +1440,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" ht="45" spans="1:6">
+    <row r="3" ht="60" spans="1:6">
       <c r="A3" s="3" t="s">
         <v>6</v>
       </c>
@@ -1394,315 +1460,295 @@
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" ht="45" spans="1:6">
       <c r="A4" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="4"/>
-      <c r="C4" s="5"/>
-      <c r="D4" s="5"/>
-      <c r="E4" s="5"/>
-      <c r="F4" s="5"/>
-    </row>
-    <row r="5" spans="1:6">
-      <c r="A5" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B5" s="4"/>
-      <c r="C5" s="5"/>
-      <c r="D5" s="5"/>
-      <c r="E5" s="5"/>
-      <c r="F5" s="5"/>
-    </row>
-    <row r="6" ht="75" spans="1:6">
+      <c r="B4" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="F4" s="5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="5" ht="45" spans="1:6">
+      <c r="A5" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="F5" s="5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" ht="60" spans="1:6">
       <c r="A6" s="6" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>18</v>
+        <v>26</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>19</v>
+        <v>27</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>20</v>
+        <v>28</v>
       </c>
       <c r="E6" s="5" t="s">
-        <v>21</v>
+        <v>29</v>
       </c>
       <c r="F6" s="5" t="s">
-        <v>22</v>
+        <v>30</v>
       </c>
     </row>
     <row r="7" ht="60" spans="1:6">
       <c r="A7" s="6" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>23</v>
+        <v>31</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>24</v>
+        <v>32</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>25</v>
+        <v>33</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>26</v>
+        <v>34</v>
       </c>
       <c r="F7" s="5" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="8" ht="45" spans="1:6">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="8" ht="60" spans="1:6">
       <c r="A8" s="6" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="C8" s="4" t="s">
-        <v>29</v>
+        <v>36</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>37</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="E8" s="5"/>
-      <c r="F8" s="5"/>
-    </row>
-    <row r="9" ht="30" spans="1:6">
+        <v>38</v>
+      </c>
+      <c r="E8" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="F8" s="5" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="9" ht="135" spans="1:6">
       <c r="A9" s="6" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>31</v>
+        <v>40</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>32</v>
+        <v>41</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="E9" s="5"/>
-      <c r="F9" s="5"/>
+        <v>42</v>
+      </c>
+      <c r="E9" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="F9" s="5" t="s">
+        <v>44</v>
+      </c>
     </row>
     <row r="10" ht="30" spans="1:6">
       <c r="A10" s="6" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>34</v>
+        <v>45</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>35</v>
+        <v>46</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="E10" s="5"/>
-      <c r="F10" s="5"/>
-    </row>
-    <row r="11" ht="195" spans="1:6">
-      <c r="A11" s="6" t="s">
-        <v>17</v>
+        <v>47</v>
+      </c>
+      <c r="E10" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="F10" s="5" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="11" ht="45" spans="1:6">
+      <c r="A11" s="7" t="s">
+        <v>50</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>36</v>
+        <v>51</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>37</v>
+        <v>52</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="E11" s="5" t="s">
-        <v>39</v>
-      </c>
+        <v>53</v>
+      </c>
+      <c r="E11" s="5"/>
       <c r="F11" s="5"/>
     </row>
-    <row r="12" ht="60" spans="1:6">
-      <c r="A12" s="6" t="s">
-        <v>17</v>
+    <row r="12" ht="30" spans="1:6">
+      <c r="A12" s="7" t="s">
+        <v>50</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>40</v>
+        <v>54</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>41</v>
+        <v>55</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>42</v>
+        <v>56</v>
       </c>
       <c r="E12" s="5"/>
       <c r="F12" s="5"/>
     </row>
-    <row r="13" spans="1:6">
-      <c r="A13" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="B13" s="4"/>
-      <c r="C13" s="5"/>
-      <c r="D13" s="5"/>
-      <c r="E13" s="5"/>
-      <c r="F13" s="5"/>
+    <row r="13" ht="105" spans="1:6">
+      <c r="A13" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="D13" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="E13" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="F13" s="5" t="s">
+        <v>61</v>
+      </c>
     </row>
     <row r="14" spans="1:6">
-      <c r="A14" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="B14" s="4"/>
-      <c r="C14" s="5"/>
+      <c r="A14" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>63</v>
+      </c>
       <c r="D14" s="5"/>
       <c r="E14" s="5"/>
       <c r="F14" s="5"/>
     </row>
-    <row r="15" spans="1:6">
-      <c r="A15" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="B15" s="4"/>
-      <c r="C15" s="5"/>
+    <row r="15" ht="30" spans="1:6">
+      <c r="A15" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="C15" s="5" t="s">
+        <v>65</v>
+      </c>
       <c r="D15" s="5"/>
       <c r="E15" s="5"/>
       <c r="F15" s="5"/>
     </row>
-    <row r="16" ht="45" spans="1:6">
+    <row r="16" spans="1:6">
       <c r="A16" s="7" t="s">
-        <v>43</v>
+        <v>50</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>44</v>
+        <v>66</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="D16" s="5" t="s">
-        <v>46</v>
-      </c>
+        <v>67</v>
+      </c>
+      <c r="D16" s="5"/>
       <c r="E16" s="5"/>
       <c r="F16" s="5"/>
     </row>
-    <row r="17" ht="30" spans="1:6">
+    <row r="17" spans="1:6">
       <c r="A17" s="7" t="s">
-        <v>43</v>
+        <v>50</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>47</v>
+        <v>68</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="D17" s="5" t="s">
-        <v>49</v>
-      </c>
+        <v>8</v>
+      </c>
+      <c r="D17" s="5"/>
       <c r="E17" s="5"/>
       <c r="F17" s="5"/>
     </row>
-    <row r="18" ht="75" spans="1:6">
+    <row r="18" spans="1:6">
       <c r="A18" s="7" t="s">
-        <v>43</v>
+        <v>50</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>50</v>
+        <v>69</v>
       </c>
       <c r="C18" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="D18" s="5" t="s">
-        <v>52</v>
-      </c>
+        <v>70</v>
+      </c>
+      <c r="D18" s="5"/>
       <c r="E18" s="5"/>
       <c r="F18" s="5"/>
     </row>
-    <row r="19" spans="1:6">
-      <c r="A19" s="7" t="s">
-        <v>43</v>
-      </c>
-      <c r="B19" s="4"/>
-      <c r="C19" s="5"/>
+    <row r="19" ht="30" spans="1:6">
+      <c r="A19" s="8" t="s">
+        <v>71</v>
+      </c>
+      <c r="B19" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="C19" s="5" t="s">
+        <v>73</v>
+      </c>
       <c r="D19" s="5"/>
       <c r="E19" s="5"/>
       <c r="F19" s="5"/>
     </row>
-    <row r="20" spans="1:6">
-      <c r="A20" s="7" t="s">
-        <v>43</v>
-      </c>
-      <c r="B20" s="4"/>
-      <c r="C20" s="5"/>
+    <row r="20" ht="30" spans="1:6">
+      <c r="A20" s="8" t="s">
+        <v>71</v>
+      </c>
+      <c r="B20" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="C20" s="5" t="s">
+        <v>75</v>
+      </c>
       <c r="D20" s="5"/>
       <c r="E20" s="5"/>
       <c r="F20" s="5"/>
-    </row>
-    <row r="21" spans="1:6">
-      <c r="A21" s="7" t="s">
-        <v>43</v>
-      </c>
-      <c r="B21" s="4"/>
-      <c r="C21" s="5"/>
-      <c r="D21" s="5"/>
-      <c r="E21" s="5"/>
-      <c r="F21" s="5"/>
-    </row>
-    <row r="22" spans="1:6">
-      <c r="A22" s="7" t="s">
-        <v>43</v>
-      </c>
-      <c r="B22" s="4"/>
-      <c r="C22" s="5"/>
-      <c r="D22" s="5"/>
-      <c r="E22" s="5"/>
-      <c r="F22" s="5"/>
-    </row>
-    <row r="23" spans="1:6">
-      <c r="A23" s="7" t="s">
-        <v>43</v>
-      </c>
-      <c r="B23" s="4"/>
-      <c r="C23" s="5"/>
-      <c r="D23" s="5"/>
-      <c r="E23" s="5"/>
-      <c r="F23" s="5"/>
-    </row>
-    <row r="24" spans="1:6">
-      <c r="A24" s="7" t="s">
-        <v>43</v>
-      </c>
-      <c r="B24" s="4"/>
-      <c r="C24" s="5"/>
-      <c r="D24" s="5"/>
-      <c r="E24" s="5"/>
-      <c r="F24" s="5"/>
-    </row>
-    <row r="25" spans="1:6">
-      <c r="A25" s="8" t="s">
-        <v>53</v>
-      </c>
-      <c r="B25" s="4"/>
-      <c r="C25" s="5"/>
-      <c r="D25" s="5"/>
-      <c r="E25" s="5"/>
-      <c r="F25" s="5"/>
-    </row>
-    <row r="26" spans="1:6">
-      <c r="A26" s="8" t="s">
-        <v>53</v>
-      </c>
-      <c r="B26" s="4"/>
-      <c r="C26" s="5"/>
-      <c r="D26" s="5"/>
-      <c r="E26" s="5"/>
-      <c r="F26" s="5"/>
-    </row>
-    <row r="27" spans="1:6">
-      <c r="A27" s="8" t="s">
-        <v>53</v>
-      </c>
-      <c r="B27" s="4"/>
-      <c r="C27" s="5"/>
-      <c r="D27" s="5"/>
-      <c r="E27" s="5"/>
-      <c r="F27" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
ajout fichier plan test
</commit_message>
<xml_diff>
--- a/Plan test.xlsx
+++ b/Plan test.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="86">
   <si>
     <t>Fichier JS</t>
   </si>
@@ -43,7 +43,7 @@
     <t>function(response)</t>
   </si>
   <si>
-    <t>récupère la réponse du serveur sous format JSON</t>
+    <t>Récupère la réponse du serveur sous format JSON</t>
   </si>
   <si>
     <t xml:space="preserve">faire un console.log(response.json) </t>
@@ -62,9 +62,6 @@
   </si>
   <si>
     <t>faire un console.log (listOfProducts) et comparer les informations contenues sur la page index.html avec les informations contenues sur l'API</t>
-  </si>
-  <si>
-    <t>un des identifiants</t>
   </si>
   <si>
     <t>16</t>
@@ -180,13 +177,10 @@
     <t>récupere les informations concernant les articles contenus dans locale storage</t>
   </si>
   <si>
-    <t>5</t>
-  </si>
-  <si>
-    <t>objArticle</t>
-  </si>
-  <si>
-    <t>transforme les données json en javascript</t>
+    <t>consulter l'onglet application de l'outil devtool</t>
+  </si>
+  <si>
+    <t>locale strorage ne s'actualise pas</t>
   </si>
   <si>
     <t>11-45</t>
@@ -200,10 +194,10 @@
 3-afficher dynamiquement les informations liés aux articles ajoutés au panier</t>
   </si>
   <si>
-    <t>ajouter plusieurs articles différents au panier et vérifier qu'ils s'affichent bien et que les monant s'actualisent bien</t>
-  </si>
-  <si>
-    <t>tous les articles ajoutés au panier ne s'affichent pas, le prix total du panier ne s'affiche pas (si par exemple les données sont de type string et pas number) ou ne s'actualise pas (s'il n'y a pas de boucle êrmettant d'additionner le prx de chaque article du panier par exemple)</t>
+    <t>ajouter plusieurs articles différents au panier et vérifier qu'ils s'affichent bien et que les monant s'actualisent bien sur la page panier</t>
+  </si>
+  <si>
+    <t>tous les articles ajoutés au panier ne s'affichent pas, le prix total du panier ne s'affiche pas (si par exemple les données sont de type string et pas number) ou ne s'actualise pas (s'il n'y a pas de boucle êrmettant d'additionner le prix de chaque article du panier par exemple)</t>
   </si>
   <si>
     <t>47-57</t>
@@ -212,40 +206,77 @@
     <t>function deleteArticle(i)</t>
   </si>
   <si>
-    <t>85-155</t>
+    <t>fonction doit supprimer la ligne de l'article concerné sur la page
+web</t>
+  </si>
+  <si>
+    <t>Cliquer sur le bouton supprimer et vérifier que l'article est supprimé sur la page et dans le locale storage</t>
+  </si>
+  <si>
+    <t>La ligne pourrait ne pas être supprimés. Il faut également veiller à ce les autre lignes non concernées ne soient pas supprimées</t>
+  </si>
+  <si>
+    <t>84-174</t>
   </si>
   <si>
     <t>myForm.addEventListener('submit',function(e)</t>
   </si>
   <si>
-    <t>123-155</t>
-  </si>
-  <si>
-    <t>function send(e)</t>
-  </si>
-  <si>
-    <t>144-148</t>
-  </si>
-  <si>
-    <t>149-152</t>
+    <t>Au clic sur le bouton "commander", vérifier la validité des données "contact" du formulaire,  envoyer au serveur les données "contact" et "products" à l'aide d'une requête de type post</t>
+  </si>
+  <si>
+    <t>Renseigner un formulaire erronné ou essayer de cliquer sur le bouton commander pour vérifier que l'envoie est bloqué puis renseigner correctement le formulaire et vérifier dans l'onglet Network de l'outil devtool qu'une réponse order a bien été transmise par le serveur</t>
+  </si>
+  <si>
+    <t>La requête pourrait contenir un chemin erroné ou présence d'erreurs bloquantes dans le formulaire pourrait bloquer la réponse du serveur</t>
+  </si>
+  <si>
+    <t>168-171</t>
   </si>
   <si>
     <t>function (orderid)</t>
   </si>
   <si>
+    <t>recupère l'order ID  envoyé par serveur et l'intègre dans l'url de la page de confirmation de commande avant d'ouvrir la page de confirmation de commande</t>
+  </si>
+  <si>
+    <t>faire un console.log (orderId) et comparer les informations contenues sur la page orderconfirmation.html le contenu de la console</t>
+  </si>
+  <si>
+    <t>la réponse du serveur pourrait ne pas avoir été reçue</t>
+  </si>
+  <si>
     <t>orderconfirmation.js</t>
   </si>
   <si>
-    <t>1-12</t>
+    <t>1-19</t>
   </si>
   <si>
     <t>document.addEventListener("DOMContentLoaded", function(event) </t>
   </si>
   <si>
-    <t>15-17</t>
+    <t>Une fois la page chargée, récupère l'orderId contenu dans le paramètre de l'url, récupère le prix total du panier dans le locale storage et affiche l'orderId et le prix total du panier sur la page</t>
+  </si>
+  <si>
+    <t>vérifier que l'orderID de l'url correspond bien à l'oderId afficher sur le DOM html et vérifier que le prix du panier correspond à celui contenu dans le localestorage</t>
+  </si>
+  <si>
+    <t>contenu du locale storage erronné ou mauvais chemin URL</t>
+  </si>
+  <si>
+    <t>22-24</t>
   </si>
   <si>
     <t>window.addEventListener("beforeunload", function (e) </t>
+  </si>
+  <si>
+    <t>fonction doit supprimer le contenu du locale storage si l'utlisateur quitte ou actualise la page</t>
+  </si>
+  <si>
+    <t>Vérifier que le locale storage est vide suite à l'actualisation ou au retour sur la page d'accueil</t>
+  </si>
+  <si>
+    <t>locale strorage ne se vide pas/la page ne se rafraichie pas</t>
   </si>
 </sst>
 </file>
@@ -253,10 +284,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_-&quot;€&quot;* #,##0_-;\-&quot;€&quot;* #,##0_-;_-&quot;€&quot;* \-_-;_-@_-"/>
-    <numFmt numFmtId="177" formatCode="_-&quot;€&quot;* #,##0.00_-;\-&quot;€&quot;* #,##0.00_-;_-&quot;€&quot;* \-??_-;_-@_-"/>
+    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="176" formatCode="_-&quot;€&quot;* #,##0.00_-;\-&quot;€&quot;* #,##0.00_-;_-&quot;€&quot;* \-??_-;_-@_-"/>
+    <numFmt numFmtId="177" formatCode="_-&quot;€&quot;* #,##0_-;\-&quot;€&quot;* #,##0_-;_-&quot;€&quot;* \-_-;_-@_-"/>
   </numFmts>
   <fonts count="21">
     <font>
@@ -281,6 +312,13 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
       <color theme="3"/>
@@ -289,6 +327,96 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <i/>
       <sz val="11"/>
       <color rgb="FF7F7F7F"/>
@@ -297,46 +425,16 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -349,73 +447,6 @@
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="38">
     <fill>
@@ -462,31 +493,127 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -498,24 +625,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -534,72 +649,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -612,31 +661,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -680,26 +711,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FF7F7F7F"/>
       </left>
       <right style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FF7F7F7F"/>
       </right>
       <top style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FF7F7F7F"/>
       </top>
       <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -728,13 +750,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
       <top style="thin">
-        <color theme="4"/>
+        <color rgb="FFB2B2B2"/>
       </top>
-      <bottom style="double">
-        <color theme="4"/>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -748,17 +774,22 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
       <top style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color theme="4"/>
       </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
+      <bottom style="double">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -767,7 +798,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -776,139 +807,139 @@
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="24" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="23" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="7" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1110,8 +1141,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:F20" totalsRowShown="0">
-  <autoFilter ref="A1:F20"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:F17" totalsRowShown="0">
+  <autoFilter ref="A1:F17"/>
   <tableColumns count="6">
     <tableColumn id="1" name="Fichier JS" dataDxfId="0"/>
     <tableColumn id="2" name="Lignes de code testées" dataDxfId="1"/>
@@ -1382,19 +1413,19 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:F20"/>
+  <dimension ref="A1:F17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="F18" sqref="F18"/>
+      <selection pane="bottomLeft" activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelCol="5"/>
   <cols>
     <col min="1" max="1" width="20" customWidth="1"/>
     <col min="2" max="2" width="22.1428571428571" customWidth="1"/>
-    <col min="3" max="3" width="34" customWidth="1"/>
+    <col min="3" max="3" width="37.1428571428571" customWidth="1"/>
     <col min="4" max="4" width="31.8571428571429" customWidth="1"/>
     <col min="5" max="5" width="39.1428571428571" customWidth="1"/>
     <col min="6" max="6" width="43.1428571428571" customWidth="1"/>
@@ -1457,7 +1488,7 @@
         <v>15</v>
       </c>
       <c r="F3" s="5" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
     </row>
     <row r="4" ht="45" spans="1:6">
@@ -1465,33 +1496,33 @@
         <v>6</v>
       </c>
       <c r="B4" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C4" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="C4" s="5" t="s">
+      <c r="D4" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="D4" s="5" t="s">
+      <c r="E4" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="E4" s="5" t="s">
+      <c r="F4" s="5" t="s">
         <v>20</v>
-      </c>
-      <c r="F4" s="5" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="5" ht="45" spans="1:6">
       <c r="A5" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="B5" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="B5" s="4" t="s">
+      <c r="C5" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="C5" s="5" t="s">
+      <c r="D5" s="5" t="s">
         <v>24</v>
-      </c>
-      <c r="D5" s="5" t="s">
-        <v>25</v>
       </c>
       <c r="E5" s="5" t="s">
         <v>10</v>
@@ -1502,253 +1533,243 @@
     </row>
     <row r="6" ht="60" spans="1:6">
       <c r="A6" s="6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B6" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C6" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="C6" s="5" t="s">
+      <c r="D6" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="D6" s="5" t="s">
+      <c r="E6" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="E6" s="5" t="s">
+      <c r="F6" s="5" t="s">
         <v>29</v>
-      </c>
-      <c r="F6" s="5" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="7" ht="60" spans="1:6">
       <c r="A7" s="6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B7" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="C7" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="C7" s="5" t="s">
+      <c r="D7" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="D7" s="5" t="s">
+      <c r="E7" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="E7" s="5" t="s">
+      <c r="F7" s="5" t="s">
         <v>34</v>
-      </c>
-      <c r="F7" s="5" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="8" ht="60" spans="1:6">
       <c r="A8" s="6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B8" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="C8" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="C8" s="5" t="s">
+      <c r="D8" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="D8" s="5" t="s">
+      <c r="E8" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="E8" s="5" t="s">
-        <v>39</v>
-      </c>
       <c r="F8" s="5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="9" ht="135" spans="1:6">
       <c r="A9" s="6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B9" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="C9" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="C9" s="5" t="s">
+      <c r="D9" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="D9" s="5" t="s">
+      <c r="E9" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="E9" s="5" t="s">
+      <c r="F9" s="5" t="s">
         <v>43</v>
-      </c>
-      <c r="F9" s="5" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="10" ht="30" spans="1:6">
       <c r="A10" s="6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B10" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="C10" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="C10" s="5" t="s">
+      <c r="D10" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="D10" s="5" t="s">
+      <c r="E10" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="E10" s="5" t="s">
+      <c r="F10" s="5" t="s">
         <v>48</v>
-      </c>
-      <c r="F10" s="5" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="11" ht="45" spans="1:6">
       <c r="A11" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="B11" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="B11" s="4" t="s">
+      <c r="C11" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="C11" s="5" t="s">
+      <c r="D11" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="D11" s="5" t="s">
+      <c r="E11" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="E11" s="5"/>
-      <c r="F11" s="5"/>
+      <c r="F11" s="5" t="s">
+        <v>54</v>
+      </c>
     </row>
-    <row r="12" ht="30" spans="1:6">
+    <row r="12" ht="105" spans="1:6">
       <c r="A12" s="7" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="E12" s="5"/>
-      <c r="F12" s="5"/>
+        <v>57</v>
+      </c>
+      <c r="E12" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="F12" s="5" t="s">
+        <v>59</v>
+      </c>
     </row>
-    <row r="13" ht="105" spans="1:6">
+    <row r="13" ht="45" spans="1:6">
       <c r="A13" s="7" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="D13" s="5" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="E13" s="5" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="F13" s="5" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
     </row>
-    <row r="14" spans="1:6">
+    <row r="14" ht="105" spans="1:6">
       <c r="A14" s="7" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="D14" s="5"/>
-      <c r="E14" s="5"/>
-      <c r="F14" s="5"/>
+        <v>66</v>
+      </c>
+      <c r="D14" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="E14" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="F14" s="5" t="s">
+        <v>69</v>
+      </c>
     </row>
-    <row r="15" ht="30" spans="1:6">
+    <row r="15" ht="75" spans="1:6">
       <c r="A15" s="7" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>64</v>
+        <v>70</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>65</v>
-      </c>
-      <c r="D15" s="5"/>
-      <c r="E15" s="5"/>
-      <c r="F15" s="5"/>
+        <v>71</v>
+      </c>
+      <c r="D15" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="E15" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="F15" s="5" t="s">
+        <v>74</v>
+      </c>
     </row>
-    <row r="16" spans="1:6">
-      <c r="A16" s="7" t="s">
-        <v>50</v>
+    <row r="16" ht="90" spans="1:6">
+      <c r="A16" s="8" t="s">
+        <v>75</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>66</v>
+        <v>76</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>67</v>
-      </c>
-      <c r="D16" s="5"/>
-      <c r="E16" s="5"/>
-      <c r="F16" s="5"/>
+        <v>77</v>
+      </c>
+      <c r="D16" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="E16" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="F16" s="5" t="s">
+        <v>80</v>
+      </c>
     </row>
-    <row r="17" spans="1:6">
-      <c r="A17" s="7" t="s">
-        <v>50</v>
+    <row r="17" ht="45" spans="1:6">
+      <c r="A17" s="8" t="s">
+        <v>75</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>68</v>
+        <v>81</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="D17" s="5"/>
-      <c r="E17" s="5"/>
-      <c r="F17" s="5"/>
-    </row>
-    <row r="18" spans="1:6">
-      <c r="A18" s="7" t="s">
-        <v>50</v>
-      </c>
-      <c r="B18" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="C18" s="5" t="s">
-        <v>70</v>
-      </c>
-      <c r="D18" s="5"/>
-      <c r="E18" s="5"/>
-      <c r="F18" s="5"/>
-    </row>
-    <row r="19" ht="30" spans="1:6">
-      <c r="A19" s="8" t="s">
-        <v>71</v>
-      </c>
-      <c r="B19" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="C19" s="5" t="s">
-        <v>73</v>
-      </c>
-      <c r="D19" s="5"/>
-      <c r="E19" s="5"/>
-      <c r="F19" s="5"/>
-    </row>
-    <row r="20" ht="30" spans="1:6">
-      <c r="A20" s="8" t="s">
-        <v>71</v>
-      </c>
-      <c r="B20" s="4" t="s">
-        <v>74</v>
-      </c>
-      <c r="C20" s="5" t="s">
-        <v>75</v>
-      </c>
-      <c r="D20" s="5"/>
-      <c r="E20" s="5"/>
-      <c r="F20" s="5"/>
+        <v>82</v>
+      </c>
+      <c r="D17" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="E17" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="F17" s="5" t="s">
+        <v>85</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
mise à jour finale
</commit_message>
<xml_diff>
--- a/Plan test.xlsx
+++ b/Plan test.xlsx
@@ -73,7 +73,7 @@
     <t>  function(response)</t>
   </si>
   <si>
-    <t xml:space="preserve">récupère la réponse du serveur avec l'id en paramètre sous format JSON </t>
+    <t>Récupère la réponse du serveur avec l'id en paramètre sous format JSON</t>
   </si>
   <si>
     <t>14-104</t>
@@ -88,7 +88,7 @@
     <t>Faire un  console.log (article) et vérifier que les informations de l'article correspondent bien aux informations de l'article cliqué</t>
   </si>
   <si>
-    <t>La requète pourrait ne pas avoir le bon format, ne pas fonctionn+er ou pourrait retourner des informations erronées</t>
+    <t>La requète pourrait ne pas avoir le bon format, ne pas fonctionner ou pourrait retourner des informations erronées</t>
   </si>
   <si>
     <t>61</t>
@@ -97,7 +97,7 @@
     <t>function showcolor()</t>
   </si>
   <si>
-    <t>permet de récupérer la couleur selectionnée par l'utilisateur</t>
+    <t>Récupère la couleur selectionnée par l'utilisateur</t>
   </si>
   <si>
     <t>Appeller la fonction avec différentes valeurs de tests, et on observe la valeur retournée, avec un console.log(getcolorSelected)</t>
@@ -113,7 +113,7 @@
     <t> function showquantity()</t>
   </si>
   <si>
-    <t>permet de récupérer la quantité selectionnée par l'utilisateur</t>
+    <t>Récupère la quantité selectionnée par l'utilisateur</t>
   </si>
   <si>
     <t>Appeller la fonction avec différentes valeurs de tests, et on observe la valeur retournée, avec un console.log(getQuantitySelected)</t>
@@ -126,10 +126,10 @@
 </t>
   </si>
   <si>
-    <t xml:space="preserve">au clic sur le bouton "ajouter au panier", récupérer les informations lié à l'article et à sa personnalisation pour les stocker dans le locale storage et afficher une pop up confirmant l'ajout de l'article au panier </t>
-  </si>
-  <si>
-    <t>Appeller la fonction avec différentes valeurs de tests (ex: ajouter différent articles ou ajouter différentes couleurs et quantités au même arrticle), et on observe la valeur retournée, avec un console.log(      console.log(selectedArticle), puis vérifier que ces éléments sont bien stockés dans le locale storage via l'onglet Application du devtool</t>
+    <t>Récupère les informations lié à l'article et à sa personnalisation pour les stocker dans le locale storage et afficher une pop up confirmant l'ajout de l'article au panier , au clic sur le bouton "ajouter au panier"</t>
+  </si>
+  <si>
+    <t>Appeller la fonction avec différentes valeurs de tests (ex: ajouter différent articles ou ajouter différentes couleurs et quantités au même arrticle), et on observe la valeur retournée, avec un console.log(selectedArticle), puis vérifier que ces éléments soient bien stockés dans le locale storage via l'onglet Application du devtool</t>
   </si>
   <si>
     <t xml:space="preserve">les articles ne sont pas stockés au locale storage ou les élements de personnalisation ne sont pas pris en compte </t>
@@ -141,7 +141,7 @@
     <t>close popup</t>
   </si>
   <si>
-    <t>ferme la pop up lorsque l'utilisateur clique sur le bouton X</t>
+    <t>Ferme la pop up lorsque l'utilisateur clique sur le bouton X</t>
   </si>
   <si>
     <t>appuyer sur la croix de la pop up et vérifier qu'elle se ferme bien</t>
@@ -159,10 +159,10 @@
     <t>getArticle</t>
   </si>
   <si>
-    <t>récupere les informations concernant les articles contenus dans locale storage</t>
-  </si>
-  <si>
-    <t>consulter l'onglet application de l'outil devtool</t>
+    <t>Récupère les informations concernant les articles contenus dans locale storage</t>
+  </si>
+  <si>
+    <t>Consulter le locale storage dans l'onglet application de l'outil devtool</t>
   </si>
   <si>
     <t>locale strorage ne s'actualise pas</t>
@@ -174,15 +174,15 @@
     <t>document.addEventListener("DOMContentLoaded", function(event)</t>
   </si>
   <si>
-    <t>une fois la page chargé, afficher la liste des articles contenus dans le locale storage (bloucle for ...of)
+    <t>Une fois la page chargée, afficher la liste des articles contenus dans le locale storage (bloucle for ...of)
 2-calculer le prix total du panier 
 3-afficher dynamiquement les informations liés aux articles ajoutés au panier</t>
   </si>
   <si>
-    <t>ajouter plusieurs articles différents au panier et vérifier qu'ils s'affichent bien et que les montants s'actualisent bien sur la page panier</t>
-  </si>
-  <si>
-    <t>tous les articles ajoutés au panier ne s'affichent pas, le prix total du panier ne s'affiche pas (si par exemple les données sont de type string et pas number) ou ne s'actualise pas (s'il n'y a pas de boucle êrmettant d'additionner le prix de chaque article du panier par exemple)</t>
+    <t>Ajouter plusieurs articles différents au panier et vérifier qu'ils s'affichent bien et que les montants s'actualisent bien sur la page panier</t>
+  </si>
+  <si>
+    <t>Tous les articles ajoutés au panier ne s'affichent pas, le prix total du panier ne s'affiche pas (si par exemple les données sont de type string et pas number) ou ne s'actualise pas (s'il n'y a pas de boucle permettant d'additionner le prix de chaque article du panier par exemple)</t>
   </si>
   <si>
     <t>47-57</t>
@@ -191,14 +191,14 @@
     <t>function deleteArticle(i)</t>
   </si>
   <si>
-    <t>fonction doit supprimer la ligne de l'article concerné sur la page
+    <t>Suprimme la ligne de l'article concerné sur la page
 web</t>
   </si>
   <si>
     <t>Cliquer sur le bouton supprimer et vérifier que l'article est supprimé sur la page et dans le locale storage</t>
   </si>
   <si>
-    <t>La ligne pourrait ne pas être supprimés. Il faut également veiller à ce les autre lignes non concernées ne soient pas supprimées</t>
+    <t>La ligne pourrait ne pas être supprimée. Il faut également veiller à ce les autre lignes non concernées ne soient pas supprimées</t>
   </si>
   <si>
     <t>84-174</t>
@@ -207,10 +207,10 @@
     <t>myForm.addEventListener('submit',function(e)</t>
   </si>
   <si>
-    <t>Au clic sur le bouton "commander", vérifier la validité des données "contact" du formulaire,  envoyer au serveur les données "contact" et "products" à l'aide d'une requête de type post</t>
-  </si>
-  <si>
-    <t>Renseigner un formulaire erronné ou essayer de cliquer sur le bouton commander pour vérifier que l'envoie est bloqué puis renseigner correctement le formulaire et vérifier dans l'onglet Network de l'outil devtool qu'une réponse order a bien été transmise par le serveur</t>
+    <t>Au clic sur le bouton "commander", vérifie la validité des données "contact" du formulaire,  envoie au serveur les données "contact" et "products" à l'aide d'une requête de type post</t>
+  </si>
+  <si>
+    <t>Renseigner un formulaire erronné et essayer de cliquer sur le bouton commander pour vérifier que l'envoi est bloqué puis renseigner correctement le formulaire et vérifier dans l'onglet Network de l'outil devtool qu'une réponse order a bien été transmise par le serveur</t>
   </si>
   <si>
     <t>La requête pourrait contenir un chemin erroné ou présence d'erreurs bloquantes dans le formulaire pourrait bloquer la réponse du serveur</t>
@@ -222,7 +222,7 @@
     <t>function (orderid)</t>
   </si>
   <si>
-    <t>recupère l'order ID  envoyé par serveur et l'intègre dans l'url de la page de confirmation de commande avant d'ouvrir la page de confirmation de commande</t>
+    <t>Récupère l'order ID  envoyé par serveur et l'intègre dans l'url de la page html "orderconfirmation" avant de l'ouvrir</t>
   </si>
   <si>
     <t>faire un console.log (orderId) et comparer les informations contenues sur la page orderconfirmation.html le contenu de la console</t>
@@ -243,7 +243,7 @@
     <t>Une fois la page chargée, récupère l'orderId contenu dans le paramètre de l'url, récupère le prix total du panier dans le locale storage et affiche l'orderId et le prix total du panier sur la page</t>
   </si>
   <si>
-    <t>vérifier que l'orderID de l'url correspond bien à l'oderId afficher sur le DOM html et vérifier que le prix du panier correspond à celui contenu dans le localestorage</t>
+    <t>Vérifier que l'orderID de l'url correspond bien à l'oderId et vérifier que le prix du panier correspond à celui contenu dans le localestorage</t>
   </si>
   <si>
     <t>contenu du locale storage erronné ou mauvais chemin URL</t>
@@ -255,7 +255,7 @@
     <t>window.addEventListener("beforeunload", function (e) </t>
   </si>
   <si>
-    <t>fonction doit supprimer le contenu du locale storage si l'utlisateur quitte ou actualise la page</t>
+    <t>Supprimme le contenu du locale storage si l'utlisateur quitte ou actualise la page</t>
   </si>
   <si>
     <t>Vérifier que le locale storage est vide suite à l'actualisation ou au retour sur la page d'accueil</t>
@@ -269,10 +269,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="176" formatCode="_-&quot;€&quot;* #,##0.00_-;\-&quot;€&quot;* #,##0.00_-;_-&quot;€&quot;* \-??_-;_-@_-"/>
+    <numFmt numFmtId="177" formatCode="_-&quot;€&quot;* #,##0_-;\-&quot;€&quot;* #,##0_-;_-&quot;€&quot;* \-_-;_-@_-"/>
+    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="176" formatCode="_-&quot;€&quot;* #,##0_-;\-&quot;€&quot;* #,##0_-;_-&quot;€&quot;* \-_-;_-@_-"/>
-    <numFmt numFmtId="177" formatCode="_-&quot;€&quot;* #,##0.00_-;\-&quot;€&quot;* #,##0.00_-;_-&quot;€&quot;* \-??_-;_-@_-"/>
   </numFmts>
   <fonts count="21">
     <font>
@@ -291,7 +291,92 @@
     <font>
       <u/>
       <sz val="11"/>
-      <color rgb="FF0000FF"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -306,6 +391,13 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -320,49 +412,17 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
+      <u/>
       <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <color rgb="FF0000FF"/>
       <name val="Calibri"/>
       <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -372,66 +432,6 @@
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="38">
     <fill>
@@ -472,12 +472,114 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -490,43 +592,37 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -544,115 +640,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -677,56 +677,6 @@
       </top>
       <bottom style="thin">
         <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -778,12 +728,62 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -792,139 +792,139 @@
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="22" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="23" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="10" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="21" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="37" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="37" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="9" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1401,9 +1401,9 @@
   <dimension ref="A1:F16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="C15" sqref="C15"/>
+      <selection pane="bottomLeft" activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelCol="5"/>
@@ -1676,7 +1676,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="14" ht="75" spans="1:6">
+    <row r="14" ht="60" spans="1:6">
       <c r="A14" s="7" t="s">
         <v>44</v>
       </c>

</xml_diff>